<commit_message>
remove raw mass at zero pressure and update plot
</commit_message>
<xml_diff>
--- a/Chapter6_Solubility-measurement/data/sorption_isotherm_data.xlsx
+++ b/Chapter6_Solubility-measurement/data/sorption_isotherm_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/sn621_ic_ac_uk/Documents/Documents/PhD Writings/25-04_PhD Thesis/Chapter6_Sorption/Figures/Python_scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="11_F25DC773A252ABDACC1048DB599F527C5BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BA36871-18B3-40CA-90C8-B3D10F2D95F3}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="11_F25DC773A252ABDACC1048DB599F527C5BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A33141C9-E9EE-4E77-BC63-4FF3B9E12DF6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48600" yWindow="-6255" windowWidth="12720" windowHeight="14805" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="16">
   <si>
     <t>T / °C</t>
   </si>
@@ -111,18 +111,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -137,13 +131,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -431,15 +421,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,360 +446,309 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>25</v>
       </c>
-      <c r="B2" s="1">
-        <v>9.9999995500000002E-6</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1.0000000000000001E-5</v>
+      <c r="B2">
+        <v>4.9653549799999999</v>
+      </c>
+      <c r="C2">
+        <v>5.0808</v>
       </c>
       <c r="D2">
-        <v>-1.6000000000460091E-5</v>
+        <v>-1.2965999999999589E-2</v>
       </c>
       <c r="E2">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>25</v>
       </c>
       <c r="B3">
-        <v>4.9653549799999999</v>
+        <v>9.5918629299999996</v>
       </c>
       <c r="C3">
-        <v>5.0808</v>
+        <v>10.044</v>
       </c>
       <c r="D3">
-        <v>-1.2965999999999589E-2</v>
+        <v>-2.6279999999999859E-2</v>
       </c>
       <c r="E3">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>25</v>
       </c>
-      <c r="B4">
-        <v>9.5918629299999996</v>
+      <c r="B4" s="1">
+        <v>18.223953999999999</v>
       </c>
       <c r="C4">
-        <v>10.044</v>
+        <v>20.03</v>
       </c>
       <c r="D4">
-        <v>-2.6279999999999859E-2</v>
+        <v>-5.6119999999999948E-2</v>
       </c>
       <c r="E4">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>25</v>
       </c>
       <c r="B5" s="1">
-        <v>18.223953999999999</v>
+        <v>25.9229284</v>
       </c>
       <c r="C5">
-        <v>20.03</v>
+        <v>29.991399999999999</v>
       </c>
       <c r="D5">
-        <v>-5.6119999999999948E-2</v>
+        <v>-9.1003999999999863E-2</v>
       </c>
       <c r="E5">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>25</v>
       </c>
       <c r="B6" s="1">
-        <v>25.9229284</v>
+        <v>32.602335500000002</v>
       </c>
       <c r="C6">
-        <v>29.991399999999999</v>
+        <v>39.812399999999997</v>
       </c>
       <c r="D6">
-        <v>-9.1003999999999863E-2</v>
+        <v>-0.1333719999999996</v>
       </c>
       <c r="E6">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>25</v>
       </c>
       <c r="B7" s="1">
-        <v>32.602335500000002</v>
+        <v>38.579752800000001</v>
       </c>
       <c r="C7">
-        <v>39.812399999999997</v>
+        <v>50.0824</v>
       </c>
       <c r="D7">
-        <v>-0.1333719999999996</v>
+        <v>-0.19112200000000001</v>
       </c>
       <c r="E7">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1">
-        <v>38.579752800000001</v>
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>4.9120149399999997</v>
       </c>
       <c r="C8">
-        <v>50.0824</v>
+        <v>5.0137999999999998</v>
       </c>
       <c r="D8">
-        <v>-0.19112200000000001</v>
+        <v>-1.2224000000000679E-2</v>
       </c>
       <c r="E8">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>35</v>
       </c>
       <c r="B9">
-        <v>9.9999995999999994E-6</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1.0000000000000001E-5</v>
+        <v>9.5864947800000007</v>
+      </c>
+      <c r="C9">
+        <v>9.9914000000000005</v>
       </c>
       <c r="D9">
-        <v>2.9799999999990945E-4</v>
+        <v>-2.5121999999999645E-2</v>
       </c>
       <c r="E9">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>35</v>
       </c>
       <c r="B10">
-        <v>4.9120149399999997</v>
+        <v>39.512771100000002</v>
       </c>
       <c r="C10">
-        <v>5.0137999999999998</v>
+        <v>49.669199999999996</v>
       </c>
       <c r="D10">
-        <v>-1.2224000000000679E-2</v>
+        <v>-0.16964999999999986</v>
       </c>
       <c r="E10">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>35</v>
       </c>
       <c r="B11">
-        <v>9.5864947800000007</v>
+        <v>39.519915699999999</v>
       </c>
       <c r="C11">
-        <v>9.9914000000000005</v>
+        <v>49.681399999999996</v>
       </c>
       <c r="D11">
-        <v>-2.5121999999999645E-2</v>
+        <v>-0.16955599999999915</v>
       </c>
       <c r="E11">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>35</v>
       </c>
       <c r="B12">
-        <v>39.512771100000002</v>
+        <v>52.67924</v>
       </c>
       <c r="C12">
-        <v>49.669199999999996</v>
+        <v>80.357600000000005</v>
       </c>
       <c r="D12">
-        <v>-0.16964999999999986</v>
+        <v>-0.57289799999999946</v>
       </c>
       <c r="E12">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>35</v>
       </c>
       <c r="B13">
-        <v>39.519915699999999</v>
+        <v>55.821534399999997</v>
       </c>
       <c r="C13">
-        <v>49.681399999999996</v>
+        <v>100.2838</v>
       </c>
       <c r="D13">
-        <v>-0.16955599999999915</v>
+        <v>-1.0852440000000003</v>
       </c>
       <c r="E13">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>35</v>
       </c>
       <c r="B14">
-        <v>52.67924</v>
+        <v>69.923960199999996</v>
       </c>
       <c r="C14">
-        <v>80.357600000000005</v>
+        <v>201.39060000000001</v>
       </c>
       <c r="D14">
-        <v>-0.57289799999999946</v>
+        <v>-1.338584</v>
       </c>
       <c r="E14">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15">
-        <v>35</v>
-      </c>
-      <c r="B15">
-        <v>55.821534399999997</v>
+        <v>50</v>
+      </c>
+      <c r="B15" s="1">
+        <v>5.0118423700000001</v>
       </c>
       <c r="C15">
-        <v>100.2838</v>
+        <v>5.1029999999999998</v>
       </c>
       <c r="D15">
-        <v>-1.0852440000000003</v>
+        <v>-1.1681999999999526E-2</v>
       </c>
       <c r="E15">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16">
-        <v>35</v>
-      </c>
-      <c r="B16">
-        <v>69.923960199999996</v>
+        <v>50</v>
+      </c>
+      <c r="B16" s="1">
+        <v>9.7781621100000002</v>
       </c>
       <c r="C16">
-        <v>201.39060000000001</v>
+        <v>10.138400000000001</v>
       </c>
       <c r="D16">
-        <v>-1.338584</v>
+        <v>-2.4144000000000609E-2</v>
       </c>
       <c r="E16">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>50</v>
       </c>
-      <c r="B17" s="3">
-        <v>9.9999996500000002E-6</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1.0000000000000001E-5</v>
+      <c r="B17" s="1">
+        <v>41.199924899999999</v>
+      </c>
+      <c r="C17">
+        <v>50.037399999999998</v>
       </c>
       <c r="D17">
-        <v>4.1000000000046555E-4</v>
+        <v>-0.15250400000000042</v>
       </c>
       <c r="E17">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>50</v>
       </c>
       <c r="B18" s="1">
-        <v>5.0118423700000001</v>
+        <v>64.3692195</v>
       </c>
       <c r="C18">
-        <v>5.1029999999999998</v>
+        <v>101.0376</v>
       </c>
       <c r="D18">
-        <v>-1.1681999999999526E-2</v>
+        <v>-0.58227799999999963</v>
       </c>
       <c r="E18">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>50</v>
       </c>
       <c r="B19" s="1">
-        <v>9.7781621100000002</v>
+        <v>84.074253799999994</v>
       </c>
       <c r="C19">
-        <v>10.138400000000001</v>
+        <v>200.8766</v>
       </c>
       <c r="D19">
-        <v>-2.4144000000000609E-2</v>
+        <v>-1.2119660000000003</v>
       </c>
       <c r="E19">
-        <v>1.5362291495737217E-4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>50</v>
-      </c>
-      <c r="B20" s="1">
-        <v>41.199924899999999</v>
-      </c>
-      <c r="C20">
-        <v>50.037399999999998</v>
-      </c>
-      <c r="D20">
-        <v>-0.15250400000000042</v>
-      </c>
-      <c r="E20">
-        <v>1.5362291495737217E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>50</v>
-      </c>
-      <c r="B21" s="1">
-        <v>64.3692195</v>
-      </c>
-      <c r="C21">
-        <v>101.0376</v>
-      </c>
-      <c r="D21">
-        <v>-0.58227799999999963</v>
-      </c>
-      <c r="E21">
-        <v>1.5362291495737217E-4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>50</v>
-      </c>
-      <c r="B22" s="1">
-        <v>84.074253799999994</v>
-      </c>
-      <c r="C22">
-        <v>200.8766</v>
-      </c>
-      <c r="D22">
-        <v>-1.2119660000000003</v>
-      </c>
-      <c r="E22">
         <v>1.5362291495737217E-4</v>
       </c>
     </row>
@@ -820,15 +759,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252820A9-3A52-49BC-9509-C6EB7725BE53}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -860,597 +799,498 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>25</v>
       </c>
       <c r="B2">
-        <v>9.9999995500000002E-6</v>
+        <v>4.9653549799999999</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>508080</v>
       </c>
       <c r="D2">
-        <f>C2*0.00001</f>
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4">
+        <f t="shared" ref="D2:D16" si="0">C2*0.00001</f>
+        <v>5.0808</v>
+      </c>
+      <c r="E2">
+        <v>1.6823759830959799E-3</v>
+      </c>
+      <c r="F2">
+        <v>1.1811780746964701E-3</v>
+      </c>
+      <c r="G2" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>4.7740521654255951E-3</v>
       </c>
       <c r="I2">
-        <v>1.8315379009622686E-4</v>
+        <v>1.8459274395816287E-4</v>
       </c>
       <c r="J2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>25</v>
       </c>
       <c r="B3">
-        <v>4.9653549799999999</v>
+        <v>9.5918629299999996</v>
       </c>
       <c r="C3">
-        <v>508080</v>
+        <v>1004400</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D19" si="0">C3*0.00001</f>
-        <v>5.0808</v>
+        <f t="shared" si="0"/>
+        <v>10.044</v>
       </c>
       <c r="E3">
-        <v>1.6823759830959799E-3</v>
+        <v>3.4613800973269299E-3</v>
       </c>
       <c r="F3">
-        <v>1.1811780746964701E-3</v>
-      </c>
-      <c r="G3" s="4">
+        <v>2.4549603781496899E-3</v>
+      </c>
+      <c r="G3" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="H3">
-        <v>4.7740521654255951E-3</v>
+        <v>9.8223044759560996E-3</v>
       </c>
       <c r="I3">
-        <v>1.8459274395816287E-4</v>
+        <v>1.887457574751694E-4</v>
       </c>
       <c r="J3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>25</v>
       </c>
       <c r="B4">
-        <v>9.5918629299999996</v>
+        <v>18.223953999999999</v>
       </c>
       <c r="C4">
-        <v>1004400</v>
+        <v>2003000</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>10.044</v>
+        <v>20.03</v>
       </c>
       <c r="E4">
-        <v>3.4613800973269299E-3</v>
+        <v>6.8360336049423298E-3</v>
       </c>
       <c r="F4">
-        <v>2.4549603781496899E-3</v>
-      </c>
-      <c r="G4" s="4">
+        <v>4.89613821036729E-3</v>
+      </c>
+      <c r="G4" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="H4">
-        <v>9.8223044759560996E-3</v>
+        <v>1.939850625693056E-2</v>
       </c>
       <c r="I4">
-        <v>1.887457574751694E-4</v>
+        <v>2.0643275470148302E-4</v>
       </c>
       <c r="J4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>25</v>
       </c>
       <c r="B5">
-        <v>18.223953999999999</v>
+        <v>25.9229284</v>
       </c>
       <c r="C5">
-        <v>2003000</v>
+        <v>2999140</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>20.03</v>
+        <v>29.991400000000002</v>
       </c>
       <c r="E5">
-        <v>6.8360336049423298E-3</v>
+        <v>1.0109266899126499E-2</v>
       </c>
       <c r="F5">
-        <v>4.89613821036729E-3</v>
-      </c>
-      <c r="G5" s="4">
+        <v>7.3050496183019297E-3</v>
+      </c>
+      <c r="G5" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="H5">
-        <v>1.939850625693056E-2</v>
+        <v>2.8686909475387337E-2</v>
       </c>
       <c r="I5">
-        <v>2.0643275470148302E-4</v>
+        <v>2.381787601017232E-4</v>
       </c>
       <c r="J5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>25</v>
       </c>
       <c r="B6">
-        <v>25.9229284</v>
+        <v>32.602335500000002</v>
       </c>
       <c r="C6">
-        <v>2999140</v>
+        <v>3981239.9999999902</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>29.991400000000002</v>
+        <v>39.812399999999904</v>
       </c>
       <c r="E6">
-        <v>1.0109266899126499E-2</v>
+        <v>1.33683528693511E-2</v>
       </c>
       <c r="F6">
-        <v>7.3050496183019297E-3</v>
-      </c>
-      <c r="G6" s="4">
+        <v>9.7418492766470095E-3</v>
+      </c>
+      <c r="G6" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="H6">
-        <v>2.8686909475387337E-2</v>
+        <v>3.793516705264216E-2</v>
       </c>
       <c r="I6">
-        <v>2.381787601017232E-4</v>
+        <v>2.8659574039788228E-4</v>
       </c>
       <c r="J6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>25</v>
       </c>
       <c r="B7">
-        <v>32.602335500000002</v>
+        <v>38.579752800000001</v>
       </c>
       <c r="C7">
-        <v>3981239.9999999902</v>
+        <v>5008240</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>39.812399999999904</v>
+        <v>50.082400000000007</v>
       </c>
       <c r="E7">
-        <v>1.33683528693511E-2</v>
+        <v>1.6342821418111698E-2</v>
       </c>
       <c r="F7">
-        <v>9.7418492766470095E-3</v>
-      </c>
-      <c r="G7" s="4">
+        <v>1.1969649685592099E-2</v>
+      </c>
+      <c r="G7" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="H7">
-        <v>3.793516705264216E-2</v>
+        <v>4.637577019895487E-2</v>
       </c>
       <c r="I7">
-        <v>2.8659574039788228E-4</v>
+        <v>3.6131331048651024E-4</v>
       </c>
       <c r="J7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B8">
-        <v>38.579752800000001</v>
+        <v>4.9120149399999997</v>
       </c>
       <c r="C8">
-        <v>5008240</v>
+        <v>501380</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>50.082400000000007</v>
+        <v>5.0138000000000007</v>
       </c>
       <c r="E8">
-        <v>1.6342821418111698E-2</v>
+        <v>1.7019651558879E-3</v>
       </c>
       <c r="F8">
-        <v>1.1969649685592099E-2</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0.64759999999999995</v>
+        <v>1.2467557305137901E-3</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.64032</v>
       </c>
       <c r="H8">
-        <v>4.637577019895487E-2</v>
+        <v>4.7318871104534586E-3</v>
       </c>
       <c r="I8">
-        <v>3.6131331048651024E-4</v>
+        <v>1.8446079372310087E-4</v>
       </c>
       <c r="J8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>35</v>
       </c>
       <c r="B9">
-        <v>9.9999995999999994E-6</v>
+        <v>9.5864947800000007</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>999140</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>9.9914000000000005</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>3.2520810986803E-3</v>
       </c>
       <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
+        <v>2.3841158768502699E-3</v>
+      </c>
+      <c r="G9" s="2">
         <v>0.64032</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>9.0415955812953187E-3</v>
       </c>
       <c r="I9">
-        <v>1.8315380637314645E-4</v>
+        <v>1.8825162263033266E-4</v>
       </c>
       <c r="J9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>35</v>
       </c>
       <c r="B10">
-        <v>4.9120149399999997</v>
+        <v>39.512771100000002</v>
       </c>
       <c r="C10">
-        <v>501380</v>
+        <v>4966920</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>5.0138000000000007</v>
+        <v>49.669200000000004</v>
       </c>
       <c r="E10">
-        <v>1.7019651558879E-3</v>
+        <v>1.45147044444725E-2</v>
       </c>
       <c r="F10">
-        <v>1.2467557305137901E-3</v>
-      </c>
-      <c r="G10" s="4">
+        <v>1.08808523860357E-2</v>
+      </c>
+      <c r="G10" s="2">
         <v>0.64032</v>
       </c>
       <c r="H10">
-        <v>4.7318871104534586E-3</v>
+        <v>4.035449411830655E-2</v>
       </c>
       <c r="I10">
-        <v>1.8446079372310087E-4</v>
+        <v>3.3185836923932665E-4</v>
       </c>
       <c r="J10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>35</v>
       </c>
       <c r="B11">
-        <v>9.5864947800000007</v>
+        <v>39.519915699999999</v>
       </c>
       <c r="C11">
-        <v>999140</v>
+        <v>4968140</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>9.9914000000000005</v>
+        <v>49.681400000000004</v>
       </c>
       <c r="E11">
-        <v>3.2520810986803E-3</v>
+        <v>1.45146815282352E-2</v>
       </c>
       <c r="F11">
-        <v>2.3841158768502699E-3</v>
-      </c>
-      <c r="G11" s="4">
+        <v>1.0880665184985599E-2</v>
+      </c>
+      <c r="G11" s="2">
         <v>0.64032</v>
       </c>
       <c r="H11">
-        <v>9.0415955812953187E-3</v>
+        <v>4.0354430405458185E-2</v>
       </c>
       <c r="I11">
-        <v>1.8825162263033266E-4</v>
+        <v>3.3133298329086154E-4</v>
       </c>
       <c r="J11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>35</v>
       </c>
       <c r="B12">
-        <v>39.512771100000002</v>
+        <v>52.67924</v>
       </c>
       <c r="C12">
-        <v>4966920</v>
+        <v>8035760</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>49.669200000000004</v>
+        <v>80.357600000000005</v>
       </c>
       <c r="E12">
-        <v>1.45147044444725E-2</v>
+        <v>1.04148412416107E-2</v>
       </c>
       <c r="F12">
-        <v>1.08808523860357E-2</v>
-      </c>
-      <c r="G12" s="4">
+        <v>6.7441431400483004E-3</v>
+      </c>
+      <c r="G12" s="2">
         <v>0.64032</v>
       </c>
       <c r="H12">
-        <v>4.035449411830655E-2</v>
+        <v>2.8955853096115158E-2</v>
       </c>
       <c r="I12">
-        <v>3.3185836923932665E-4</v>
+        <v>9.0822179232402775E-4</v>
       </c>
       <c r="J12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B13">
-        <v>39.519915699999999</v>
+        <v>5.0118423700000001</v>
       </c>
       <c r="C13">
-        <v>4968140</v>
+        <v>510300</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>49.681400000000004</v>
+        <v>5.1030000000000006</v>
       </c>
       <c r="E13">
-        <v>1.45146815282352E-2</v>
+        <v>1.78413284214917E-3</v>
       </c>
       <c r="F13">
-        <v>1.0880665184985599E-2</v>
-      </c>
-      <c r="G13" s="4">
-        <v>0.64032</v>
+        <v>1.3875230168461301E-3</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.62939999999999996</v>
       </c>
       <c r="H13">
-        <v>4.0354430405458185E-2</v>
+        <v>4.8141738859934424E-3</v>
       </c>
       <c r="I13">
-        <v>3.3133298329086154E-4</v>
+        <v>1.8438907664273767E-4</v>
       </c>
       <c r="J13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B14">
-        <v>52.67924</v>
+        <v>9.7781621100000002</v>
       </c>
       <c r="C14">
-        <v>8035760</v>
+        <v>1013840</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>80.357600000000005</v>
+        <v>10.138400000000001</v>
       </c>
       <c r="E14">
-        <v>1.04148412416107E-2</v>
+        <v>3.03187748613277E-3</v>
       </c>
       <c r="F14">
-        <v>6.7441431400483004E-3</v>
-      </c>
-      <c r="G14" s="4">
-        <v>0.64032</v>
+        <v>2.33383039314564E-3</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.62939999999999996</v>
       </c>
       <c r="H14">
-        <v>2.8955853096115158E-2</v>
+        <v>8.1809969944219366E-3</v>
       </c>
       <c r="I14">
-        <v>9.0822179232402775E-4</v>
+        <v>1.8785000175738394E-4</v>
       </c>
       <c r="J14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>50</v>
       </c>
       <c r="B15">
-        <v>9.9999996500000002E-6</v>
+        <v>41.199924899999999</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>5003740</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>50.037400000000005</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1.22765667178354E-2</v>
       </c>
       <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15" s="4">
+        <v>9.5059470843157894E-3</v>
+      </c>
+      <c r="G15" s="2">
         <v>0.62939999999999996</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>3.3126191899178085E-2</v>
       </c>
       <c r="I15">
-        <v>1.8315381234016597E-4</v>
+        <v>3.0836007367409659E-4</v>
       </c>
       <c r="J15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>50</v>
       </c>
       <c r="B16">
-        <v>5.0118423700000001</v>
+        <v>64.3692195</v>
       </c>
       <c r="C16">
-        <v>510300</v>
+        <v>10103760</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>5.1030000000000006</v>
+        <v>101.03760000000001</v>
       </c>
       <c r="E16">
-        <v>1.78413284214917E-3</v>
+        <v>1.0051666016538801E-2</v>
       </c>
       <c r="F16">
-        <v>1.3875230168461301E-3</v>
-      </c>
-      <c r="G16" s="4">
+        <v>6.4030563968146201E-3</v>
+      </c>
+      <c r="G16" s="2">
         <v>0.62939999999999996</v>
       </c>
       <c r="H16">
-        <v>4.8141738859934424E-3</v>
+        <v>2.7122682181702103E-2</v>
       </c>
       <c r="I16">
-        <v>1.8438907664273767E-4</v>
+        <v>9.1849135180407753E-4</v>
       </c>
       <c r="J16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>50</v>
-      </c>
-      <c r="B17">
-        <v>9.7781621100000002</v>
-      </c>
-      <c r="C17">
-        <v>1013840</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>10.138400000000001</v>
-      </c>
-      <c r="E17">
-        <v>3.03187748613277E-3</v>
-      </c>
-      <c r="F17">
-        <v>2.33383039314564E-3</v>
-      </c>
-      <c r="G17" s="4">
-        <v>0.62939999999999996</v>
-      </c>
-      <c r="H17">
-        <v>8.1809969944219366E-3</v>
-      </c>
-      <c r="I17">
-        <v>1.8785000175738394E-4</v>
-      </c>
-      <c r="J17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>50</v>
-      </c>
-      <c r="B18">
-        <v>41.199924899999999</v>
-      </c>
-      <c r="C18">
-        <v>5003740</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>50.037400000000005</v>
-      </c>
-      <c r="E18">
-        <v>1.22765667178354E-2</v>
-      </c>
-      <c r="F18">
-        <v>9.5059470843157894E-3</v>
-      </c>
-      <c r="G18" s="4">
-        <v>0.62939999999999996</v>
-      </c>
-      <c r="H18">
-        <v>3.3126191899178085E-2</v>
-      </c>
-      <c r="I18">
-        <v>3.0836007367409659E-4</v>
-      </c>
-      <c r="J18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>50</v>
-      </c>
-      <c r="B19">
-        <v>64.3692195</v>
-      </c>
-      <c r="C19">
-        <v>10103760</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>101.03760000000001</v>
-      </c>
-      <c r="E19">
-        <v>1.0051666016538801E-2</v>
-      </c>
-      <c r="F19">
-        <v>6.4030563968146201E-3</v>
-      </c>
-      <c r="G19" s="4">
-        <v>0.62939999999999996</v>
-      </c>
-      <c r="H19">
-        <v>2.7122682181702103E-2</v>
-      </c>
-      <c r="I19">
-        <v>9.1849135180407753E-4</v>
-      </c>
-      <c r="J19" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1461,15 +1301,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C813E2CF-114D-4DB6-BE54-EA0E74154A76}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1510,843 +1350,717 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>25</v>
       </c>
       <c r="B2">
-        <v>9.9999995500000002E-6</v>
+        <v>4.9653549799999999</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>508080</v>
       </c>
       <c r="D2">
-        <f>C2*0.00001</f>
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>7.99549820291128E-7</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1.1826985323632701E-6</v>
+        <f t="shared" ref="D2:D18" si="0">C2*0.00001</f>
+        <v>5.0808</v>
+      </c>
+      <c r="E2">
+        <v>1.70457446499335E-3</v>
+      </c>
+      <c r="F2">
+        <v>1.20093910434609E-3</v>
+      </c>
+      <c r="G2">
+        <v>8.1029327818212105E-7</v>
+      </c>
+      <c r="H2">
+        <v>1.18228839417002E-6</v>
       </c>
       <c r="I2">
-        <v>950478.83049795299</v>
-      </c>
-      <c r="J2" s="4">
+        <v>950960.607045535</v>
+      </c>
+      <c r="J2" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>4.83704445230803E-3</v>
       </c>
       <c r="L2">
-        <v>1.822768331245517E-4</v>
+        <v>1.8396208103137017E-4</v>
       </c>
       <c r="M2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>25</v>
       </c>
       <c r="B3">
-        <v>4.9653549799999999</v>
+        <v>9.5918629299999996</v>
       </c>
       <c r="C3">
-        <v>508080</v>
+        <v>1004400</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D21" si="0">C3*0.00001</f>
-        <v>5.0808</v>
+        <f t="shared" si="0"/>
+        <v>10.044</v>
       </c>
       <c r="E3">
-        <v>1.70457446499335E-3</v>
+        <v>3.5564133813253398E-3</v>
       </c>
       <c r="F3">
-        <v>1.20093910434609E-3</v>
+        <v>2.5289672847137999E-3</v>
       </c>
       <c r="G3">
-        <v>8.1029327818212105E-7</v>
+        <v>8.19361150897454E-7</v>
       </c>
       <c r="H3">
-        <v>1.18228839417002E-6</v>
+        <v>1.1818152173647399E-6</v>
       </c>
       <c r="I3">
-        <v>950960.607045535</v>
-      </c>
-      <c r="J3" s="4">
+        <v>951456.01285964297</v>
+      </c>
+      <c r="J3" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="K3">
-        <v>4.83704445230803E-3</v>
+        <v>1.009197894814228E-2</v>
       </c>
       <c r="L3">
-        <v>1.8396208103137017E-4</v>
+        <v>1.8887432214440808E-4</v>
       </c>
       <c r="M3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>25</v>
       </c>
       <c r="B4">
-        <v>9.5918629299999996</v>
+        <v>18.223953999999999</v>
       </c>
       <c r="C4">
-        <v>1004400</v>
+        <v>2003000</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>10.044</v>
+        <v>20.03</v>
       </c>
       <c r="E4">
-        <v>3.5564133813253398E-3</v>
+        <v>7.1389386986849103E-3</v>
       </c>
       <c r="F4">
-        <v>2.5289672847137999E-3</v>
+        <v>5.13852287873007E-3</v>
       </c>
       <c r="G4">
-        <v>8.19361150897454E-7</v>
+        <v>8.3744761441118902E-7</v>
       </c>
       <c r="H4">
-        <v>1.1818152173647399E-6</v>
+        <v>1.1806970951528599E-6</v>
       </c>
       <c r="I4">
-        <v>951456.01285964297</v>
-      </c>
-      <c r="J4" s="4">
+        <v>952373.40237711999</v>
+      </c>
+      <c r="J4" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="K4">
-        <v>1.009197894814228E-2</v>
+        <v>2.0258055331114952E-2</v>
       </c>
       <c r="L4">
-        <v>1.8887432214440808E-4</v>
+        <v>2.0969736987168038E-4</v>
       </c>
       <c r="M4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>25</v>
       </c>
       <c r="B5">
-        <v>18.223953999999999</v>
+        <v>25.9229284</v>
       </c>
       <c r="C5">
-        <v>2003000</v>
+        <v>2999140</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>20.03</v>
+        <v>29.991400000000002</v>
       </c>
       <c r="E5">
-        <v>7.1389386986849103E-3</v>
+        <v>1.07647093247666E-2</v>
       </c>
       <c r="F5">
-        <v>5.13852287873007E-3</v>
+        <v>7.8351924374013907E-3</v>
       </c>
       <c r="G5">
-        <v>8.3744761441118902E-7</v>
+        <v>8.5378456987386898E-7</v>
       </c>
       <c r="H5">
-        <v>1.1806970951528599E-6</v>
+        <v>1.17938129965203E-6</v>
       </c>
       <c r="I5">
-        <v>952373.40237711999</v>
-      </c>
-      <c r="J5" s="4">
+        <v>953244.66291806905</v>
+      </c>
+      <c r="J5" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="K5">
-        <v>2.0258055331114952E-2</v>
+        <v>3.0546848254161742E-2</v>
       </c>
       <c r="L5">
-        <v>2.0969736987168038E-4</v>
+        <v>2.4658276910879571E-4</v>
       </c>
       <c r="M5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>25</v>
       </c>
       <c r="B6">
-        <v>25.9229284</v>
+        <v>32.602335500000002</v>
       </c>
       <c r="C6">
-        <v>2999140</v>
+        <v>3981239.9999999902</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>29.991400000000002</v>
+        <v>39.812399999999904</v>
       </c>
       <c r="E6">
-        <v>1.07647093247666E-2</v>
+        <v>1.3947508934990201E-2</v>
       </c>
       <c r="F6">
-        <v>7.8351924374013907E-3</v>
+        <v>1.02195914943859E-2</v>
       </c>
       <c r="G6">
-        <v>8.5378456987386898E-7</v>
+        <v>8.6674571402676404E-7</v>
       </c>
       <c r="H6">
-        <v>1.17938129965203E-6</v>
+        <v>1.1780152049147E-6</v>
       </c>
       <c r="I6">
-        <v>953244.66291806905</v>
-      </c>
-      <c r="J6" s="4">
+        <v>953989.29659005802</v>
+      </c>
+      <c r="J6" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="K6">
-        <v>3.0546848254161742E-2</v>
+        <v>3.9578629213933597E-2</v>
       </c>
       <c r="L6">
-        <v>2.4658276910879571E-4</v>
+        <v>3.0136416088890347E-4</v>
       </c>
       <c r="M6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>25</v>
       </c>
       <c r="B7">
-        <v>32.602335500000002</v>
+        <v>38.579752800000001</v>
       </c>
       <c r="C7">
-        <v>3981239.9999999902</v>
+        <v>5008240</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>39.812399999999904</v>
+        <v>50.082400000000007</v>
       </c>
       <c r="E7">
-        <v>1.3947508934990201E-2</v>
+        <v>1.8398992415628101E-2</v>
       </c>
       <c r="F7">
-        <v>1.02195914943859E-2</v>
+        <v>1.36869664032224E-2</v>
       </c>
       <c r="G7">
-        <v>8.6674571402676404E-7</v>
+        <v>8.8361245009645297E-7</v>
       </c>
       <c r="H7">
-        <v>1.1780152049147E-6</v>
+        <v>1.17618913740569E-6</v>
       </c>
       <c r="I7">
-        <v>953989.29659005802</v>
-      </c>
-      <c r="J7" s="4">
+        <v>954900.12389419205</v>
+      </c>
+      <c r="J7" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="K7">
-        <v>3.9578629213933597E-2</v>
+        <v>5.2210534664097898E-2</v>
       </c>
       <c r="L7">
-        <v>3.0136416088890347E-4</v>
+        <v>3.8632309539899946E-4</v>
       </c>
       <c r="M7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B8">
-        <v>38.579752800000001</v>
+        <v>4.9120149399999997</v>
       </c>
       <c r="C8">
-        <v>5008240</v>
+        <v>501380</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>50.082400000000007</v>
+        <v>5.0138000000000007</v>
       </c>
       <c r="E8">
-        <v>1.8398992415628101E-2</v>
+        <v>1.76030706068877E-3</v>
       </c>
       <c r="F8">
-        <v>1.36869664032224E-2</v>
+        <v>1.2915917045192701E-3</v>
       </c>
       <c r="G8">
-        <v>8.8361245009645297E-7</v>
+        <v>8.3946817300536704E-7</v>
       </c>
       <c r="H8">
-        <v>1.17618913740569E-6</v>
+        <v>1.19022506384466E-6</v>
       </c>
       <c r="I8">
-        <v>954900.12389419205</v>
-      </c>
-      <c r="J8" s="4">
-        <v>0.64759999999999995</v>
+        <v>950926.74068310799</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.64032</v>
       </c>
       <c r="K8">
-        <v>5.2210534664097898E-2</v>
+        <v>4.8940921393704684E-3</v>
       </c>
       <c r="L8">
-        <v>3.8632309539899946E-4</v>
+        <v>1.8382045258895688E-4</v>
       </c>
       <c r="M8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>35</v>
       </c>
       <c r="B9">
-        <v>9.9999995999999994E-6</v>
+        <v>9.5864947800000007</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>999140</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>9.9914000000000005</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>3.4119789170306402E-3</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>2.5135650950346301E-3</v>
       </c>
       <c r="G9">
-        <v>8.3030173645617104E-7</v>
+        <v>8.4937383830852999E-7</v>
       </c>
       <c r="H9">
-        <v>1.19066277175029E-6</v>
+        <v>1.1897317518561799E-6</v>
       </c>
       <c r="I9">
-        <v>950551.94826830796</v>
-      </c>
-      <c r="J9" s="4">
+        <v>951333.69390536204</v>
+      </c>
+      <c r="J9" s="2">
         <v>0.64032</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>9.4861513485060053E-3</v>
       </c>
       <c r="L9">
-        <v>1.822768331245517E-4</v>
+        <v>1.8833124442913497E-4</v>
       </c>
       <c r="M9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>35</v>
       </c>
       <c r="B10">
-        <v>4.9120149399999997</v>
+        <v>39.512771100000002</v>
       </c>
       <c r="C10">
-        <v>501380</v>
+        <v>4966920</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>5.0138000000000007</v>
+        <v>49.669200000000004</v>
       </c>
       <c r="E10">
-        <v>1.76030706068877E-3</v>
+        <v>1.6118193973491901E-2</v>
       </c>
       <c r="F10">
-        <v>1.2915917045192701E-3</v>
+        <v>1.22572730036116E-2</v>
       </c>
       <c r="G10">
-        <v>8.3946817300536704E-7</v>
+        <v>9.0725544974417704E-7</v>
       </c>
       <c r="H10">
-        <v>1.19022506384466E-6</v>
+        <v>1.1843378073265601E-6</v>
       </c>
       <c r="I10">
-        <v>950926.74068310799</v>
-      </c>
-      <c r="J10" s="4">
+        <v>954107.17251125199</v>
+      </c>
+      <c r="J10" s="2">
         <v>0.64032</v>
       </c>
       <c r="K10">
-        <v>4.8940921393704684E-3</v>
+        <v>4.4812594454770635E-2</v>
       </c>
       <c r="L10">
-        <v>1.8382045258895688E-4</v>
+        <v>3.5306501822053945E-4</v>
       </c>
       <c r="M10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>35</v>
       </c>
       <c r="B11">
-        <v>9.5864947800000007</v>
+        <v>39.519915699999999</v>
       </c>
       <c r="C11">
-        <v>999140</v>
+        <v>4968140</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>9.9914000000000005</v>
+        <v>49.681400000000004</v>
       </c>
       <c r="E11">
-        <v>3.4119789170306402E-3</v>
+        <v>1.6118175056795699E-2</v>
       </c>
       <c r="F11">
-        <v>2.5135650950346301E-3</v>
+        <v>1.2257119494484299E-2</v>
       </c>
       <c r="G11">
-        <v>8.4937383830852999E-7</v>
+        <v>9.07243129264944E-7</v>
       </c>
       <c r="H11">
-        <v>1.1897317518561799E-6</v>
+        <v>1.18433687801041E-6</v>
       </c>
       <c r="I11">
-        <v>951333.69390536204</v>
-      </c>
-      <c r="J11" s="4">
+        <v>954107.57552837604</v>
+      </c>
+      <c r="J11" s="2">
         <v>0.64032</v>
       </c>
       <c r="K11">
-        <v>9.4861513485060053E-3</v>
+        <v>4.4812541861642845E-2</v>
       </c>
       <c r="L11">
-        <v>1.8833124442913497E-4</v>
+        <v>3.5340533499556405E-4</v>
       </c>
       <c r="M11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>35</v>
       </c>
       <c r="B12">
-        <v>39.512771100000002</v>
+        <v>52.67924</v>
       </c>
       <c r="C12">
-        <v>4966920</v>
+        <v>8035760</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>49.669200000000004</v>
+        <v>80.357600000000005</v>
       </c>
       <c r="E12">
-        <v>1.6118193973491901E-2</v>
+        <v>0.39792237180640699</v>
       </c>
       <c r="F12">
-        <v>1.22572730036116E-2</v>
+        <v>0.42806978486901398</v>
       </c>
       <c r="G12">
-        <v>9.0725544974417704E-7</v>
+        <v>1.2493920779189399E-6</v>
       </c>
       <c r="H12">
-        <v>1.1843378073265601E-6</v>
+        <v>1.0194265330511099E-6</v>
       </c>
       <c r="I12">
-        <v>954107.17251125199</v>
-      </c>
-      <c r="J12" s="4">
+        <v>930416.55005519697</v>
+      </c>
+      <c r="J12" s="2">
         <v>0.64032</v>
       </c>
       <c r="K12">
-        <v>4.4812594454770635E-2</v>
+        <v>1.1063233201913005</v>
       </c>
       <c r="L12">
-        <v>3.5306501822053945E-4</v>
+        <v>1.2290487290588866E-3</v>
       </c>
       <c r="M12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>35</v>
       </c>
       <c r="B13">
-        <v>39.519915699999999</v>
+        <v>55.821534399999997</v>
       </c>
       <c r="C13">
-        <v>4968140</v>
+        <v>10028380</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>49.681400000000004</v>
+        <v>100.28380000000001</v>
       </c>
       <c r="E13">
-        <v>1.6118175056795699E-2</v>
+        <v>0.109604316297594</v>
       </c>
       <c r="F13">
-        <v>1.2257119494484299E-2</v>
+        <v>0.10143594945666</v>
       </c>
       <c r="G13">
-        <v>9.07243129264944E-7</v>
+        <v>1.0903654922217E-6</v>
       </c>
       <c r="H13">
-        <v>1.18433687801041E-6</v>
+        <v>1.1438594822309299E-6</v>
       </c>
       <c r="I13">
-        <v>954107.57552837604</v>
-      </c>
-      <c r="J13" s="4">
+        <v>957530.73943021195</v>
+      </c>
+      <c r="J13" s="2">
         <v>0.64032</v>
       </c>
       <c r="K13">
-        <v>4.4812541861642845E-2</v>
+        <v>0.3047273028736488</v>
       </c>
       <c r="L13">
-        <v>3.5340533499556405E-4</v>
+        <v>1.8550326320006384E-3</v>
       </c>
       <c r="M13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>35</v>
       </c>
       <c r="B14">
-        <v>52.67924</v>
+        <v>69.923960199999996</v>
       </c>
       <c r="C14">
-        <v>8035760</v>
+        <v>20139060</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>80.357600000000005</v>
+        <v>201.39060000000001</v>
       </c>
       <c r="E14">
-        <v>0.39792237180640699</v>
+        <v>3.2130027472381702E-2</v>
       </c>
       <c r="F14">
-        <v>0.42806978486901398</v>
+        <v>2.2677042649622101E-2</v>
       </c>
       <c r="G14">
-        <v>1.2493920779189399E-6</v>
+        <v>9.2992513153251001E-7</v>
       </c>
       <c r="H14">
-        <v>1.0194265330511099E-6</v>
+        <v>1.1686282986698299E-6</v>
       </c>
       <c r="I14">
-        <v>930416.55005519697</v>
-      </c>
-      <c r="J14" s="4">
+        <v>959267.57842734898</v>
+      </c>
+      <c r="J14" s="2">
         <v>0.64032</v>
       </c>
       <c r="K14">
-        <v>1.1063233201913005</v>
+        <v>8.9329480294655539E-2</v>
       </c>
       <c r="L14">
-        <v>1.2290487290588866E-3</v>
+        <v>2.242401800507957E-3</v>
       </c>
       <c r="M14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B15">
-        <v>55.821534399999997</v>
+        <v>5.0118423700000001</v>
       </c>
       <c r="C15">
-        <v>10028380</v>
+        <v>510300</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>100.28380000000001</v>
+        <v>5.1030000000000006</v>
       </c>
       <c r="E15">
-        <v>0.109604316297594</v>
+        <v>1.8270977669058699E-3</v>
       </c>
       <c r="F15">
-        <v>0.10143594945666</v>
+        <v>1.42197519972843E-3</v>
       </c>
       <c r="G15">
-        <v>1.0903654922217E-6</v>
+        <v>8.8717306859472902E-7</v>
       </c>
       <c r="H15">
-        <v>1.1438594822309299E-6</v>
+        <v>1.2023153120420901E-6</v>
       </c>
       <c r="I15">
-        <v>957530.73943021195</v>
-      </c>
-      <c r="J15" s="4">
-        <v>0.64032</v>
+        <v>950866.402085618</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.62939999999999996</v>
       </c>
       <c r="K15">
-        <v>0.3047273028736488</v>
+        <v>4.930107304117296E-3</v>
       </c>
       <c r="L15">
-        <v>1.8550326320006384E-3</v>
+        <v>1.8372775057618656E-4</v>
       </c>
       <c r="M15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A16">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B16">
-        <v>69.923960199999996</v>
+        <v>9.7781621100000002</v>
       </c>
       <c r="C16">
-        <v>20139060</v>
+        <v>1013840</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>201.39060000000001</v>
+        <v>10.138400000000001</v>
       </c>
       <c r="E16">
-        <v>3.2130027472381702E-2</v>
+        <v>3.1747692372162402E-3</v>
       </c>
       <c r="F16">
-        <v>2.2677042649622101E-2</v>
+        <v>2.4559722869304601E-3</v>
       </c>
       <c r="G16">
-        <v>9.2992513153251001E-7</v>
+        <v>8.9550171255609503E-7</v>
       </c>
       <c r="H16">
-        <v>1.1686282986698299E-6</v>
+        <v>1.20179280403797E-6</v>
       </c>
       <c r="I16">
-        <v>959267.57842734898</v>
-      </c>
-      <c r="J16" s="4">
-        <v>0.64032</v>
+        <v>951163.44795238401</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.62939999999999996</v>
       </c>
       <c r="K16">
-        <v>8.9329480294655539E-2</v>
+        <v>8.5665656697685912E-3</v>
       </c>
       <c r="L16">
-        <v>2.242401800507957E-3</v>
+        <v>1.8784349984668527E-4</v>
       </c>
       <c r="M16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>50</v>
       </c>
       <c r="B17">
-        <v>9.9999996500000002E-6</v>
+        <v>41.199924899999999</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>5003740</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>50.037400000000005</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1.2511544963814399E-2</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>9.7170668235394102E-3</v>
       </c>
       <c r="G17">
-        <v>8.7859801504870698E-7</v>
+        <v>9.4074251229889897E-7</v>
       </c>
       <c r="H17">
-        <v>1.2027974722368E-6</v>
+        <v>1.19678061483758E-6</v>
       </c>
       <c r="I17">
-        <v>950559.03795363102</v>
-      </c>
-      <c r="J17" s="4">
+        <v>953112.31277268403</v>
+      </c>
+      <c r="J17" s="2">
         <v>0.62939999999999996</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>3.3760240053465729E-2</v>
       </c>
       <c r="L17">
-        <v>1.822768331245517E-4</v>
+        <v>3.2530006745144931E-4</v>
       </c>
       <c r="M17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>50</v>
       </c>
       <c r="B18">
-        <v>5.0118423700000001</v>
+        <v>64.3692195</v>
       </c>
       <c r="C18">
-        <v>510300</v>
+        <v>10103760</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>5.1030000000000006</v>
+        <v>101.03760000000001</v>
       </c>
       <c r="E18">
-        <v>1.8270977669058699E-3</v>
+        <v>2.4331241859107199E-2</v>
       </c>
       <c r="F18">
-        <v>1.42197519972843E-3</v>
+        <v>1.9279487158111501E-2</v>
       </c>
       <c r="G18">
-        <v>8.8717306859472902E-7</v>
+        <v>9.800818024891971E-7</v>
       </c>
       <c r="H18">
-        <v>1.2023153120420901E-6</v>
+        <v>1.1889327529373201E-6</v>
       </c>
       <c r="I18">
-        <v>950866.402085618</v>
-      </c>
-      <c r="J18" s="4">
+        <v>955192.71706303</v>
+      </c>
+      <c r="J18" s="2">
         <v>0.62939999999999996</v>
       </c>
       <c r="K18">
-        <v>4.930107304117296E-3</v>
+        <v>6.565364775797948E-2</v>
       </c>
       <c r="L18">
-        <v>1.8372775057618656E-4</v>
+        <v>1.0053041926798014E-3</v>
       </c>
       <c r="M18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>50</v>
-      </c>
-      <c r="B19">
-        <v>9.7781621100000002</v>
-      </c>
-      <c r="C19">
-        <v>1013840</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>10.138400000000001</v>
-      </c>
-      <c r="E19">
-        <v>3.1747692372162402E-3</v>
-      </c>
-      <c r="F19">
-        <v>2.4559722869304601E-3</v>
-      </c>
-      <c r="G19">
-        <v>8.9550171255609503E-7</v>
-      </c>
-      <c r="H19">
-        <v>1.20179280403797E-6</v>
-      </c>
-      <c r="I19">
-        <v>951163.44795238401</v>
-      </c>
-      <c r="J19" s="4">
-        <v>0.62939999999999996</v>
-      </c>
-      <c r="K19">
-        <v>8.5665656697685912E-3</v>
-      </c>
-      <c r="L19">
-        <v>1.8784349984668527E-4</v>
-      </c>
-      <c r="M19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>50</v>
-      </c>
-      <c r="B20">
-        <v>41.199924899999999</v>
-      </c>
-      <c r="C20">
-        <v>5003740</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>50.037400000000005</v>
-      </c>
-      <c r="E20">
-        <v>1.2511544963814399E-2</v>
-      </c>
-      <c r="F20">
-        <v>9.7170668235394102E-3</v>
-      </c>
-      <c r="G20">
-        <v>9.4074251229889897E-7</v>
-      </c>
-      <c r="H20">
-        <v>1.19678061483758E-6</v>
-      </c>
-      <c r="I20">
-        <v>953112.31277268403</v>
-      </c>
-      <c r="J20" s="4">
-        <v>0.62939999999999996</v>
-      </c>
-      <c r="K20">
-        <v>3.3760240053465729E-2</v>
-      </c>
-      <c r="L20">
-        <v>3.2530006745144931E-4</v>
-      </c>
-      <c r="M20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>50</v>
-      </c>
-      <c r="B21">
-        <v>64.3692195</v>
-      </c>
-      <c r="C21">
-        <v>10103760</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>101.03760000000001</v>
-      </c>
-      <c r="E21">
-        <v>2.4331241859107199E-2</v>
-      </c>
-      <c r="F21">
-        <v>1.9279487158111501E-2</v>
-      </c>
-      <c r="G21">
-        <v>9.800818024891971E-7</v>
-      </c>
-      <c r="H21">
-        <v>1.1889327529373201E-6</v>
-      </c>
-      <c r="I21">
-        <v>955192.71706303</v>
-      </c>
-      <c r="J21" s="4">
-        <v>0.62939999999999996</v>
-      </c>
-      <c r="K21">
-        <v>6.565364775797948E-2</v>
-      </c>
-      <c r="L21">
-        <v>1.0053041926798014E-3</v>
-      </c>
-      <c r="M21" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2357,26 +2071,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3804D1B7-9B6C-492F-9FD6-82689F2CDE59}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.4609375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.3046875" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2408,597 +2122,498 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>25</v>
       </c>
       <c r="B2">
-        <v>9.9999995500000002E-6</v>
+        <v>4.9653549799999999</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>508080</v>
       </c>
       <c r="D2">
-        <f>C2*0.00001</f>
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4">
+        <f t="shared" ref="D2:D16" si="0">C2*0.00001</f>
+        <v>5.0808</v>
+      </c>
+      <c r="E2">
+        <v>1.65524700528166E-3</v>
+      </c>
+      <c r="F2">
+        <v>1.16092627549507E-3</v>
+      </c>
+      <c r="G2" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>4.6970686869513617E-3</v>
       </c>
       <c r="I2">
-        <v>1.822768331245517E-4</v>
+        <v>1.8394945157882515E-4</v>
       </c>
       <c r="J2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>25</v>
       </c>
       <c r="B3">
-        <v>4.9653549799999999</v>
+        <v>9.5918629299999996</v>
       </c>
       <c r="C3">
-        <v>508080</v>
+        <v>1004400</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D19" si="0">C3*0.00001</f>
-        <v>5.0808</v>
+        <f t="shared" si="0"/>
+        <v>10.044</v>
       </c>
       <c r="E3">
-        <v>1.65524700528166E-3</v>
+        <v>3.3774883253155298E-3</v>
       </c>
       <c r="F3">
-        <v>1.16092627549507E-3</v>
-      </c>
-      <c r="G3" s="4">
+        <v>2.3900468611849999E-3</v>
+      </c>
+      <c r="G3" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="H3">
-        <v>4.6970686869513617E-3</v>
+        <v>9.5842460990792546E-3</v>
       </c>
       <c r="I3">
-        <v>1.8394945157882515E-4</v>
+        <v>1.8879802158832973E-4</v>
       </c>
       <c r="J3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>25</v>
       </c>
       <c r="B4">
-        <v>9.5918629299999996</v>
+        <v>18.223953999999999</v>
       </c>
       <c r="C4">
-        <v>1004400</v>
+        <v>2003000</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>10.044</v>
+        <v>20.03</v>
       </c>
       <c r="E4">
-        <v>3.3774883253155298E-3</v>
+        <v>6.4552198403203401E-3</v>
       </c>
       <c r="F4">
-        <v>2.3900468611849999E-3</v>
-      </c>
-      <c r="G4" s="4">
+        <v>4.5949079627247598E-3</v>
+      </c>
+      <c r="G4" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="H4">
-        <v>9.5842460990792546E-3</v>
+        <v>1.8317876958911291E-2</v>
       </c>
       <c r="I4">
-        <v>1.8879802158832973E-4</v>
+        <v>2.0920159511149213E-4</v>
       </c>
       <c r="J4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>25</v>
       </c>
       <c r="B5">
-        <v>18.223953999999999</v>
+        <v>25.9229284</v>
       </c>
       <c r="C5">
-        <v>2003000</v>
+        <v>2999140</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>20.03</v>
+        <v>29.991400000000002</v>
       </c>
       <c r="E5">
-        <v>6.4552198403203401E-3</v>
+        <v>9.2497661686680808E-3</v>
       </c>
       <c r="F5">
-        <v>4.5949079627247598E-3</v>
-      </c>
-      <c r="G5" s="4">
+        <v>6.6108885348348601E-3</v>
+      </c>
+      <c r="G5" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="H5">
-        <v>1.8317876958911291E-2</v>
+        <v>2.624791761824086E-2</v>
       </c>
       <c r="I5">
-        <v>2.0920159511149213E-4</v>
+        <v>2.4516425155594613E-4</v>
       </c>
       <c r="J5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>25</v>
       </c>
       <c r="B6">
-        <v>25.9229284</v>
+        <v>32.602335500000002</v>
       </c>
       <c r="C6">
-        <v>2999140</v>
+        <v>3981239.9999999902</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>29.991400000000002</v>
+        <v>39.812399999999904</v>
       </c>
       <c r="E6">
-        <v>9.2497661686680808E-3</v>
+        <v>1.1088111164623901E-2</v>
       </c>
       <c r="F6">
-        <v>6.6108885348348601E-3</v>
-      </c>
-      <c r="G6" s="4">
+        <v>7.8811091742312309E-3</v>
+      </c>
+      <c r="G6" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="H6">
-        <v>2.624791761824086E-2</v>
+        <v>3.1464560626061011E-2</v>
       </c>
       <c r="I6">
-        <v>2.4516425155594613E-4</v>
+        <v>2.9833204944140258E-4</v>
       </c>
       <c r="J6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>25</v>
       </c>
       <c r="B7">
-        <v>32.602335500000002</v>
+        <v>38.579752800000001</v>
       </c>
       <c r="C7">
-        <v>3981239.9999999902</v>
+        <v>5008240</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>39.812399999999904</v>
+        <v>50.082400000000007</v>
       </c>
       <c r="E7">
-        <v>1.1088111164623901E-2</v>
+        <v>1.2955578022193199E-2</v>
       </c>
       <c r="F7">
-        <v>7.8811091742312309E-3</v>
-      </c>
-      <c r="G7" s="4">
+        <v>9.1758167069618708E-3</v>
+      </c>
+      <c r="G7" s="2">
         <v>0.64759999999999995</v>
       </c>
       <c r="H7">
-        <v>3.1464560626061011E-2</v>
+        <v>3.67638422877219E-2</v>
       </c>
       <c r="I7">
-        <v>2.9833204944140258E-4</v>
+        <v>3.8024255865052946E-4</v>
       </c>
       <c r="J7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B8">
-        <v>38.579752800000001</v>
+        <v>4.9120149399999997</v>
       </c>
       <c r="C8">
-        <v>5008240</v>
+        <v>501380</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>50.082400000000007</v>
+        <v>5.0138000000000007</v>
       </c>
       <c r="E8">
-        <v>1.2955578022193199E-2</v>
+        <v>1.7236861831265301E-3</v>
       </c>
       <c r="F8">
-        <v>9.1758167069618708E-3</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0.64759999999999995</v>
+        <v>1.26338466232395E-3</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.64032</v>
       </c>
       <c r="H8">
-        <v>3.67638422877219E-2</v>
+        <v>4.7922769771089023E-3</v>
       </c>
       <c r="I8">
-        <v>3.8024255865052946E-4</v>
+        <v>1.8381138028130098E-4</v>
       </c>
       <c r="J8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>35</v>
       </c>
       <c r="B9">
-        <v>9.9999995999999994E-6</v>
+        <v>9.5864947800000007</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>999140</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>9.9914000000000005</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>3.28226440829289E-3</v>
       </c>
       <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
+        <v>2.4085022583098898E-3</v>
+      </c>
+      <c r="G9" s="2">
         <v>0.64032</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>9.1255127009922422E-3</v>
       </c>
       <c r="I9">
-        <v>1.822768331245517E-4</v>
+        <v>1.8827774498894107E-4</v>
       </c>
       <c r="J9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>35</v>
       </c>
       <c r="B10">
-        <v>4.9120149399999997</v>
+        <v>39.512771100000002</v>
       </c>
       <c r="C10">
-        <v>501380</v>
+        <v>4966920</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>5.0138000000000007</v>
+        <v>49.669200000000004</v>
       </c>
       <c r="E10">
-        <v>1.7236861831265301E-3</v>
+        <v>1.36093388485927E-2</v>
       </c>
       <c r="F10">
-        <v>1.26338466232395E-3</v>
-      </c>
-      <c r="G10" s="4">
+        <v>1.01073329962736E-2</v>
+      </c>
+      <c r="G10" s="2">
         <v>0.64032</v>
       </c>
       <c r="H10">
-        <v>4.7922769771089023E-3</v>
+        <v>3.7837352225847144E-2</v>
       </c>
       <c r="I10">
-        <v>1.8381138028130098E-4</v>
+        <v>3.5030377462924009E-4</v>
       </c>
       <c r="J10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>35</v>
       </c>
       <c r="B11">
-        <v>9.5864947800000007</v>
+        <v>39.519915699999999</v>
       </c>
       <c r="C11">
-        <v>999140</v>
+        <v>4968140</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>9.9914000000000005</v>
+        <v>49.681400000000004</v>
       </c>
       <c r="E11">
-        <v>3.28226440829289E-3</v>
+        <v>1.3609483527042599E-2</v>
       </c>
       <c r="F11">
-        <v>2.4085022583098898E-3</v>
-      </c>
-      <c r="G11" s="4">
+        <v>1.0108519322275199E-2</v>
+      </c>
+      <c r="G11" s="2">
         <v>0.64032</v>
       </c>
       <c r="H11">
-        <v>9.1255127009922422E-3</v>
+        <v>3.7837754467978754E-2</v>
       </c>
       <c r="I11">
-        <v>1.8827774498894107E-4</v>
+        <v>3.5039662617712209E-4</v>
       </c>
       <c r="J11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>35</v>
       </c>
       <c r="B12">
-        <v>39.512771100000002</v>
+        <v>52.67924</v>
       </c>
       <c r="C12">
-        <v>4966920</v>
+        <v>8035760</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>49.669200000000004</v>
+        <v>80.357600000000005</v>
       </c>
       <c r="E12">
-        <v>1.36093388485927E-2</v>
+        <v>0.253757242488174</v>
       </c>
       <c r="F12">
-        <v>1.01073329962736E-2</v>
-      </c>
-      <c r="G12" s="4">
+        <v>0.26043841488906999</v>
+      </c>
+      <c r="G12" s="2">
         <v>0.64032</v>
       </c>
       <c r="H12">
-        <v>3.7837352225847144E-2</v>
+        <v>0.70550834766507453</v>
       </c>
       <c r="I12">
-        <v>3.5030377462924009E-4</v>
+        <v>1.153396052628876E-3</v>
       </c>
       <c r="J12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B13">
-        <v>39.519915699999999</v>
+        <v>5.0118423700000001</v>
       </c>
       <c r="C13">
-        <v>4968140</v>
+        <v>510300</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>49.681400000000004</v>
+        <v>5.1030000000000006</v>
       </c>
       <c r="E13">
-        <v>1.3609483527042599E-2</v>
+        <v>1.8491906058859899E-3</v>
       </c>
       <c r="F13">
-        <v>1.0108519322275199E-2</v>
-      </c>
-      <c r="G13" s="4">
-        <v>0.64032</v>
+        <v>1.4407880404423801E-3</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.62939999999999996</v>
       </c>
       <c r="H13">
-        <v>3.7837754467978754E-2</v>
+        <v>4.9897210088666747E-3</v>
       </c>
       <c r="I13">
-        <v>3.5039662617712209E-4</v>
+        <v>1.8373309678769803E-4</v>
       </c>
       <c r="J13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B14">
-        <v>52.67924</v>
+        <v>9.7781621100000002</v>
       </c>
       <c r="C14">
-        <v>8035760</v>
+        <v>1013840</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>80.357600000000005</v>
+        <v>10.138400000000001</v>
       </c>
       <c r="E14">
-        <v>0.253757242488174</v>
+        <v>3.1899135337871698E-3</v>
       </c>
       <c r="F14">
-        <v>0.26043841488906999</v>
-      </c>
-      <c r="G14" s="4">
-        <v>0.64032</v>
+        <v>2.4691786830764099E-3</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.62939999999999996</v>
       </c>
       <c r="H14">
-        <v>0.70550834766507453</v>
+        <v>8.6074299346658653E-3</v>
       </c>
       <c r="I14">
-        <v>1.153396052628876E-3</v>
+        <v>1.8784955367454542E-4</v>
       </c>
       <c r="J14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>50</v>
       </c>
       <c r="B15">
-        <v>9.9999996500000002E-6</v>
+        <v>41.199924899999999</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>5003740</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>1.0000000000000001E-5</v>
+        <v>50.037400000000005</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1.3024803230138699E-2</v>
       </c>
       <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15" s="4">
+        <v>1.01773275016321E-2</v>
+      </c>
+      <c r="G15" s="2">
         <v>0.62939999999999996</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>3.5145178710573932E-2</v>
       </c>
       <c r="I15">
-        <v>1.822768331245517E-4</v>
+        <v>3.2585375279381521E-4</v>
       </c>
       <c r="J15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>50</v>
       </c>
       <c r="B16">
-        <v>5.0118423700000001</v>
+        <v>64.3692195</v>
       </c>
       <c r="C16">
-        <v>510300</v>
+        <v>10103760</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>5.1030000000000006</v>
+        <v>101.03760000000001</v>
       </c>
       <c r="E16">
-        <v>1.8491906058859899E-3</v>
+        <v>6.50463158997618E-2</v>
       </c>
       <c r="F16">
-        <v>1.4407880404423801E-3</v>
-      </c>
-      <c r="G16" s="4">
+        <v>5.9625737808877997E-2</v>
+      </c>
+      <c r="G16" s="2">
         <v>0.62939999999999996</v>
       </c>
       <c r="H16">
-        <v>4.9897210088666747E-3</v>
+        <v>0.17551623286498055</v>
       </c>
       <c r="I16">
-        <v>1.8373309678769803E-4</v>
+        <v>1.0383387727153329E-3</v>
       </c>
       <c r="J16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>50</v>
-      </c>
-      <c r="B17">
-        <v>9.7781621100000002</v>
-      </c>
-      <c r="C17">
-        <v>1013840</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>10.138400000000001</v>
-      </c>
-      <c r="E17">
-        <v>3.1899135337871698E-3</v>
-      </c>
-      <c r="F17">
-        <v>2.4691786830764099E-3</v>
-      </c>
-      <c r="G17" s="4">
-        <v>0.62939999999999996</v>
-      </c>
-      <c r="H17">
-        <v>8.6074299346658653E-3</v>
-      </c>
-      <c r="I17">
-        <v>1.8784955367454542E-4</v>
-      </c>
-      <c r="J17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>50</v>
-      </c>
-      <c r="B18">
-        <v>41.199924899999999</v>
-      </c>
-      <c r="C18">
-        <v>5003740</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>50.037400000000005</v>
-      </c>
-      <c r="E18">
-        <v>1.3024803230138699E-2</v>
-      </c>
-      <c r="F18">
-        <v>1.01773275016321E-2</v>
-      </c>
-      <c r="G18" s="4">
-        <v>0.62939999999999996</v>
-      </c>
-      <c r="H18">
-        <v>3.5145178710573932E-2</v>
-      </c>
-      <c r="I18">
-        <v>3.2585375279381521E-4</v>
-      </c>
-      <c r="J18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>50</v>
-      </c>
-      <c r="B19">
-        <v>64.3692195</v>
-      </c>
-      <c r="C19">
-        <v>10103760</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>101.03760000000001</v>
-      </c>
-      <c r="E19">
-        <v>6.50463158997618E-2</v>
-      </c>
-      <c r="F19">
-        <v>5.9625737808877997E-2</v>
-      </c>
-      <c r="G19" s="4">
-        <v>0.62939999999999996</v>
-      </c>
-      <c r="H19">
-        <v>0.17551623286498055</v>
-      </c>
-      <c r="I19">
-        <v>1.0383387727153329E-3</v>
-      </c>
-      <c r="J19" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>